<commit_message>
Redo naming of mixres units
</commit_message>
<xml_diff>
--- a/outputs/density_geounits/summary_stats_Clermont.xlsx
+++ b/outputs/density_geounits/summary_stats_Clermont.xlsx
@@ -7,11 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="area_mixres" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="area_mixres_new" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="area_hires" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="area_lores" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="area_pop_sum" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="area_mixre" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="area_hires" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="area_lores" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="area_pop_sum" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -457,7 +456,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>83</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
@@ -467,7 +466,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.74898989221566</v>
+        <v>4.644271060505967</v>
       </c>
     </row>
     <row r="4">
@@ -477,7 +476,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.376944421311559</v>
+        <v>8.099524446477252</v>
       </c>
     </row>
     <row r="5">
@@ -487,7 +486,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.06207961225517048</v>
+        <v>0.2052519461442788</v>
       </c>
     </row>
     <row r="6">
@@ -497,7 +496,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.6340618503335815</v>
+        <v>0.8763157409606921</v>
       </c>
     </row>
     <row r="7">
@@ -507,7 +506,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.566124774558961</v>
+        <v>2.953657468676412</v>
       </c>
     </row>
     <row r="8">
@@ -517,7 +516,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4.248712733025812</v>
+        <v>5.247786480337977</v>
       </c>
     </row>
     <row r="9">
@@ -568,7 +567,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>67</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
@@ -578,7 +577,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.644271060505967</v>
+        <v>2.430985633233592</v>
       </c>
     </row>
     <row r="4">
@@ -588,7 +587,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8.099524446477252</v>
+        <v>6.107117444246778</v>
       </c>
     </row>
     <row r="5">
@@ -598,7 +597,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2052519461442788</v>
+        <v>0.06207961225517048</v>
       </c>
     </row>
     <row r="6">
@@ -608,7 +607,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8763157409606921</v>
+        <v>0.3763391941996322</v>
       </c>
     </row>
     <row r="7">
@@ -618,7 +617,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.953657468676412</v>
+        <v>0.6932829408665976</v>
       </c>
     </row>
     <row r="8">
@@ -628,7 +627,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.247786480337977</v>
+        <v>2.610917105963219</v>
       </c>
     </row>
     <row r="9">
@@ -679,7 +678,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>128</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
@@ -689,7 +688,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.430985633233592</v>
+        <v>16.37716859067474</v>
       </c>
     </row>
     <row r="4">
@@ -699,7 +698,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.107117444246778</v>
+        <v>21.12303719069318</v>
       </c>
     </row>
     <row r="5">
@@ -709,7 +708,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.06207961225517048</v>
+        <v>0.65412270206793</v>
       </c>
     </row>
     <row r="6">
@@ -719,7 +718,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.3763391941996322</v>
+        <v>4.292223242007331</v>
       </c>
     </row>
     <row r="7">
@@ -729,7 +728,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.6932829408665976</v>
+        <v>10.39167996499148</v>
       </c>
     </row>
     <row r="8">
@@ -739,7 +738,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.610917105963219</v>
+        <v>21.38839530726406</v>
       </c>
     </row>
     <row r="9">
@@ -749,7 +748,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>51.81788468825613</v>
+        <v>94.6155244803208</v>
       </c>
     </row>
   </sheetData>
@@ -758,117 +757,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>index</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>area</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>count</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>mean</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>16.37716859067474</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>std</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>21.12303719069318</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>min</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.65412270206793</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>4.292223242007331</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>50%</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>10.39167996499148</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>75%</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>21.38839530726406</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>max</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>94.6155244803208</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
create summary tables and figures
</commit_message>
<xml_diff>
--- a/outputs/density_geounits/summary_stats_Clermont.xlsx
+++ b/outputs/density_geounits/summary_stats_Clermont.xlsx
@@ -762,7 +762,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -779,11 +779,6 @@
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Density</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -794,20 +789,24 @@
       <c r="B2" t="n">
         <v>311.1662032228199</v>
       </c>
-      <c r="C2" t="n">
-        <v>915.362905900288</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Population</t>
+          <t>population</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>284830</v>
       </c>
-      <c r="C3" t="n">
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>density</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>915.362905900288</v>
       </c>
     </row>

</xml_diff>

<commit_message>
redo FR pop dens calcs using overlays
</commit_message>
<xml_diff>
--- a/outputs/density_geounits/summary_stats_Clermont.xlsx
+++ b/outputs/density_geounits/summary_stats_Clermont.xlsx
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>284830</v>
+        <v>284405</v>
       </c>
     </row>
     <row r="4">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>915.362905900288</v>
+        <v>913.9970763352575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>